<commit_message>
DEBUG: always upload new ppp grade after the old one deleted
</commit_message>
<xml_diff>
--- a/basketBallRecorder/spreadsheet_for_defense.xlsx
+++ b/basketBallRecorder/spreadsheet_for_defense.xlsx
@@ -264,14 +264,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -612,34 +612,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:T23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
@@ -706,521 +709,521 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="12"/>
-      <c r="T20" s="12"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" spans="2:20">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" spans="2:20">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" spans="2:20">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
     </row>
     <row r="26" spans="2:20">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
     </row>
     <row r="27" spans="2:20">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>